<commit_message>
recherche des dossiers en utilisant button browse et monter le emplacement dans textbox(textBox_Research)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA6EED-3E4C-4043-8D85-0506D5DA925C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B563EF9A-7ADF-49CD-BBB9-9E48A484C148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Auteur:</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>journal de travail mis à jour</t>
+  </si>
+  <si>
+    <t>construction du winforms en ajoutant chque element nécessaire</t>
+  </si>
+  <si>
+    <t>DataGridView pour afficher Local media files  catalog et Global media files  catalog</t>
+  </si>
+  <si>
+    <t>recherche des dossiers en utilisant button browse et monter le emplacement dans textbox(textBox_Research)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/32450856/how-i-can-make-a-button-for-browse-a-folder</t>
   </si>
 </sst>
 </file>
@@ -425,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -632,6 +644,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1179,7 +1202,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2112,13 +2135,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>0.62857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65</c:v>
+                  <c:v>0.37142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4307,7 +4330,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4362,7 +4385,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 40 minutes</v>
+        <v>2 heures 55 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4381,11 +4404,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4584,16 +4607,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="str">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="63">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="B13" s="34">
+        <v>45975</v>
+      </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="23"/>
+      <c r="D13" s="36">
+        <v>25</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>38</v>
+      </c>
       <c r="G13" s="84"/>
       <c r="N13">
         <v>6</v>
@@ -4603,16 +4634,26 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="str">
+      <c r="A14" s="62">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="B14" s="30">
+        <v>45975</v>
+      </c>
       <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="39"/>
+      <c r="D14" s="36">
+        <v>20</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="85" t="s">
+        <v>41</v>
+      </c>
       <c r="N14">
         <v>7</v>
       </c>
@@ -4620,17 +4661,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="str">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="63">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="34">
+        <v>45975</v>
+      </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="40"/>
+      <c r="D15" s="32">
+        <v>30</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="84"/>
       <c r="N15">
         <v>8</v>
       </c>
@@ -4638,27 +4687,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="str">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="62">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="B16" s="30">
+        <v>45975</v>
+      </c>
       <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="23"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="91"/>
       <c r="G16" s="39"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45975</v>
+      </c>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
       <c r="E17" s="37"/>
@@ -4669,11 +4722,13 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45975</v>
+      </c>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
       <c r="E18" s="33"/>
@@ -4698,7 +4753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="str">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
         <v/>
@@ -4722,7 +4777,7 @@
       <c r="F21" s="23"/>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="str">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
         <v/>
@@ -4770,7 +4825,7 @@
       <c r="F25" s="23"/>
       <c r="G25" s="84"/>
     </row>
-    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="str">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
         <v/>
@@ -4818,7 +4873,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="40"/>
     </row>
-    <row r="30" spans="1:15" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="str">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
         <v/>
@@ -10862,7 +10917,7 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E532">
+  <conditionalFormatting sqref="E17:E532 E7:E15">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>$E7="Absent"</formula>
     </cfRule>
@@ -10895,10 +10950,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D15 D17:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
       <formula1>$O$7:$O$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{EBCA439E-C5F1-BC4C-88EE-2BB045537E3E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E15 E17:E532" xr:uid="{EBCA439E-C5F1-BC4C-88EE-2BB045537E3E}">
       <formula1>$M$7:$M$12</formula1>
     </dataValidation>
   </dataValidations>
@@ -10908,11 +10963,12 @@
     <hyperlink ref="G10" r:id="rId3" display="https://www.coingecko.com/en/api?" xr:uid="{0F91120E-3455-4E0F-8C60-6729CE2C909C}"/>
     <hyperlink ref="G20" r:id="rId4" display="https://scottplot.net/cookbook/4.1/category/plottable-scatter-plot/" xr:uid="{4AC877DD-0538-4960-9300-3F6AF2D7E0D5}"/>
     <hyperlink ref="G31" r:id="rId5" display="https://gist.github.com/takekazuomi/10955889" xr:uid="{14778DBD-AC08-49BE-B816-D74CEFC0A64E}"/>
+    <hyperlink ref="G14" r:id="rId6" xr:uid="{64AB34B8-9A53-4FFA-8DD1-6FAFB9B69698}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11041,11 +11097,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11053,11 +11109,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 35 min</v>
+        <v>1 h 50 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.35</v>
+        <v>0.62857142857142856</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11131,7 +11187,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.65</v>
+        <v>0.37142857142857144</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11187,22 +11243,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 40 min</v>
+        <v>2 h 55 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>6.9444444444444448E-2</v>
+        <v>0.12152777777777778</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11246,6 +11302,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11446,15 +11511,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11467,6 +11523,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11485,14 +11549,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix(StyleDataGrid), feat(extensions de fichiers possibles (wav, ogg, mp3))
correction stylistique-esthétique de dataGrid ;
différentes extensions de fichiers possibles (wav, ogg, mp3);
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EC0074-C610-49D2-9AFB-01D448AC1096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E10C18-6190-47D8-9EB6-B9C2F58F489E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Auteur:</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>stylisation des datagrids</t>
+  </si>
+  <si>
+    <t>correction stylistique-esthétique de grid dans application, pour avoir une correspendance entre maquette et application réel</t>
+  </si>
+  <si>
+    <t>Implémentation des différentes extensions de fichiers possibles (wav, ogg, mp3), ajout d’un DataMusic pour chaque extension.</t>
   </si>
 </sst>
 </file>
@@ -1215,13 +1221,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2148,13 +2154,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.70175438596491224</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.2982456140350877</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4343,7 +4349,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4398,7 +4404,7 @@
       <c r="B3" s="92"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 45 minutes</v>
+        <v>4 heures 45 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4417,11 +4423,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>225</v>
+        <v>285</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>225</v>
+        <v>285</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4773,39 +4779,57 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+    <row r="19" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45982</v>
+      </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>20</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" s="84"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45982</v>
+      </c>
       <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+      <c r="D20" s="32">
+        <v>30</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="G20" s="89"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45982</v>
+      </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
       <c r="E21" s="37"/>
@@ -4813,11 +4837,13 @@
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45982</v>
+      </c>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
@@ -4825,11 +4851,13 @@
       <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="str">
+      <c r="A23" s="63">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B23" s="34">
+        <v>45982</v>
+      </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
       <c r="E23" s="37"/>
@@ -4837,15 +4865,23 @@
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="str">
+      <c r="A24" s="62">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B24" s="30">
+        <v>45982</v>
+      </c>
       <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="23"/>
+      <c r="D24" s="32">
+        <v>10</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -11132,11 +11168,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11144,11 +11180,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 30 min</v>
+        <v>3 h 20 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.66666666666666663</v>
+        <v>0.70175438596491224</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11206,11 +11242,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11218,11 +11254,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 15 min</v>
+        <v>1 h 25 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.2982456140350877</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11278,22 +11314,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>225</v>
+        <v>285</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>225</v>
+        <v>285</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 45 min</v>
+        <v>4 h 45 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.15625</v>
+        <v>0.19791666666666666</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11337,6 +11373,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11537,15 +11582,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11558,6 +11594,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11576,14 +11620,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat(type tag est ajouté "featuring"), chore(JDT)
(nouveau type de tag est ajouté "featuring" dans la dataGrid), journal de travail mis à jour
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CE692-D780-4FE3-AC5D-2E72B50B153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520CE408-CD50-4F3B-B6F2-FCAA08E47F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Auteur:</t>
   </si>
@@ -187,13 +187,16 @@
     <t>Implémentation des différentes extensions de fichiers possibles (wav, ogg, mp3), ajout d’un DataMusic pour chaque extension.</t>
   </si>
   <si>
-    <t>download files from dataGrid</t>
-  </si>
-  <si>
     <t xml:space="preserve"> https://www.codeproject.com/articles/Upload-and-Download-Files-From-DataGridView-Cells#comments-section </t>
   </si>
   <si>
     <t>correction de maquette, ajout de maquette.pdf, palette des couleurs</t>
+  </si>
+  <si>
+    <t>nouveau type de tag est ajouté "featuring" dans la dataGrid</t>
+  </si>
+  <si>
+    <t>download files from dataGrid [wip]</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>240</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2163,13 +2166,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7384615384615385</c:v>
+                  <c:v>0.75362318840579712</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26153846153846155</c:v>
+                  <c:v>0.24637681159420291</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4358,7 +4361,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4413,7 +4416,7 @@
       <c r="B3" s="92"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 25 minutes</v>
+        <v>5 heures 45 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4432,11 +4435,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4841,16 +4844,16 @@
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="40" t="s">
         <v>48</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -4869,7 +4872,7 @@
         <v>19</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="39"/>
     </row>
@@ -4882,9 +4885,15 @@
         <v>45982</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+      <c r="D23" s="36">
+        <v>25</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -11191,11 +11200,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11203,11 +11212,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 00 min</v>
+        <v>4 h 20 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.7384615384615385</v>
+        <v>0.75362318840579712</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11281,7 +11290,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.26153846153846155</v>
+        <v>0.24637681159420291</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11337,22 +11346,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 25 min</v>
+        <v>5 h 45 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.22569444444444445</v>
+        <v>0.23958333333333334</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11396,15 +11405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11605,6 +11605,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11617,14 +11626,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11643,6 +11644,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
test(music_data new song added)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520CE408-CD50-4F3B-B6F2-FCAA08E47F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945AA70B-210B-472E-A9E2-B148EC85805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Auteur:</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>download files from dataGrid [wip]</t>
+  </si>
+  <si>
+    <t>sous-total du jour [28.11.2025]: 2h15</t>
+  </si>
+  <si>
+    <t>music data added new songs for testing</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1239,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2166,13 +2172,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75362318840579712</c:v>
+                  <c:v>0.76388888888888884</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24637681159420291</c:v>
+                  <c:v>0.2361111111111111</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4361,7 +4367,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4416,7 +4422,7 @@
       <c r="B3" s="92"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 45 minutes</v>
+        <v>6 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4435,11 +4441,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4917,23 +4923,33 @@
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="str">
+      <c r="A25" s="63">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B25" s="34">
+        <v>45989</v>
+      </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="23"/>
+      <c r="D25" s="36">
+        <v>15</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G25" s="84"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="62" t="str">
+      <c r="A26" s="62">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B26" s="30">
+        <v>45989</v>
+      </c>
       <c r="C26" s="31"/>
       <c r="D26" s="32"/>
       <c r="E26" s="33"/>
@@ -4941,11 +4957,13 @@
       <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="str">
+      <c r="A27" s="63">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B27" s="34">
+        <v>45989</v>
+      </c>
       <c r="C27" s="35"/>
       <c r="D27" s="36"/>
       <c r="E27" s="37"/>
@@ -4953,11 +4971,13 @@
       <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="str">
+      <c r="A28" s="62">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B28" s="30">
+        <v>45989</v>
+      </c>
       <c r="C28" s="31"/>
       <c r="D28" s="32"/>
       <c r="E28" s="33"/>
@@ -4965,11 +4985,13 @@
       <c r="G28" s="39"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="63" t="str">
+      <c r="A29" s="63">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B29" s="34">
+        <v>45989</v>
+      </c>
       <c r="C29" s="35"/>
       <c r="D29" s="36"/>
       <c r="E29" s="37"/>
@@ -4977,11 +4999,13 @@
       <c r="G29" s="40"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="62" t="str">
+      <c r="A30" s="62">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B30" s="30">
+        <v>45989</v>
+      </c>
       <c r="C30" s="31"/>
       <c r="D30" s="32"/>
       <c r="E30" s="33"/>
@@ -4989,15 +5013,19 @@
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="63" t="str">
+      <c r="A31" s="63">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B31" s="34">
+        <v>45989</v>
+      </c>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
       <c r="E31" s="37"/>
-      <c r="F31" s="22"/>
+      <c r="F31" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="G31" s="84"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -11200,11 +11228,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11212,11 +11240,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 20 min</v>
+        <v>4 h 35 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.75362318840579712</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11290,7 +11318,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.24637681159420291</v>
+        <v>0.2361111111111111</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11346,22 +11374,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 45 min</v>
+        <v>6 h 00 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.23958333333333334</v>
+        <v>0.25</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11405,6 +11433,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11605,15 +11642,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11626,6 +11654,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11644,14 +11680,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
MQTT C#  transferring mp3 by chunks (FileTransferService,NetworkProtocol), planing of functionement and understanding of details
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945AA70B-210B-472E-A9E2-B148EC85805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31016209-D74B-4950-9C59-AC8D4C936AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="4665" yWindow="0" windowWidth="21600" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>Auteur:</t>
   </si>
@@ -203,6 +203,23 @@
   </si>
   <si>
     <t>music data added new songs for testing</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7UewJo4zY2k</t>
+  </si>
+  <si>
+    <t>MQTT C#  transferring mp3 by chunks (FileTransferService,NetworkProtocol), planing of functionement and understanding of details</t>
+  </si>
+  <si>
+    <t>feat(NetworkProtocol)</t>
+  </si>
+  <si>
+    <t>AskMedia() 
+SendMedia()
+AskCatalog()
+SendCatalog()
+SayOnline()
+GetOnlineMediatheque()</t>
   </si>
 </sst>
 </file>
@@ -1239,13 +1256,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2172,13 +2189,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76388888888888884</c:v>
+                  <c:v>0.78409090909090906</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2361111111111111</c:v>
+                  <c:v>0.21590909090909091</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4366,8 +4383,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4422,7 +4439,7 @@
       <c r="B3" s="92"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 0 minutes</v>
+        <v>7 heures 20 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4441,11 +4458,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4942,7 +4959,7 @@
       </c>
       <c r="G25" s="84"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="62">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
         <v>48</v>
@@ -4951,12 +4968,20 @@
         <v>45989</v>
       </c>
       <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D26" s="32">
+        <v>20</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A27" s="63">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
         <v>48</v>
@@ -4965,10 +4990,18 @@
         <v>45989</v>
       </c>
       <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="40"/>
+      <c r="D27" s="36">
+        <v>50</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="62">
@@ -5007,9 +5040,15 @@
         <v>45989</v>
       </c>
       <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="23"/>
+      <c r="D30" s="32">
+        <v>10</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -11228,11 +11267,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>275</v>
+        <v>345</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>345</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11240,11 +11279,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 35 min</v>
+        <v>5 h 45 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.76388888888888884</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11302,11 +11341,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11314,11 +11353,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 25 min</v>
+        <v>1 h 35 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.2361111111111111</v>
+        <v>0.21590909090909091</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11374,22 +11413,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 00 min</v>
+        <v>7 h 20 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.25</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11433,15 +11472,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11642,6 +11672,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11654,14 +11693,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11680,6 +11711,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix((NetworkProtocol.cs) bugs with version of mqttnet, and implementation of features functions for messages transfer + comments); chore(JDT)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E50C9EB-56ED-4FAE-A01E-73A1A9E66DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2E2653-953C-4287-A1BE-A408385DC017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>Auteur:</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>feat(NetworkProtocol)[WIP] NetworkProtocol ALL methods + configuration of broker;</t>
+  </si>
+  <si>
+    <t>fix(NetworkProtocol.cs) bugs with version of mqttnet, and implementation of features functions for messages transfer + comments</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1278,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>515</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2208,13 +2211,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83739837398373984</c:v>
+                  <c:v>0.85915492957746475</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16260162601626016</c:v>
+                  <c:v>0.14084507042253522</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4403,7 +4406,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4458,7 +4461,7 @@
       <c r="B3" s="92"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>10 heures 15 minutes</v>
+        <v>11 heures 50 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4473,15 +4476,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>555</v>
+        <v>590</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>615</v>
+        <v>710</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5179,15 +5182,25 @@
       <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="str">
+      <c r="A36" s="62">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="22"/>
+        <v>51</v>
+      </c>
+      <c r="B36" s="30">
+        <v>46008</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1</v>
+      </c>
+      <c r="D36" s="32">
+        <v>35</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>64</v>
+      </c>
       <c r="G36" s="39"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -11326,15 +11339,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>455</v>
+        <v>490</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>515</v>
+        <v>610</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11342,11 +11355,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>8 h 35 min</v>
+        <v>10 h 10 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.83739837398373984</v>
+        <v>0.85915492957746475</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11420,7 +11433,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.16260162601626016</v>
+        <v>0.14084507042253522</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11472,26 +11485,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>555</v>
+        <v>590</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>615</v>
+        <v>710</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>10 h 15 min</v>
+        <v>11 h 50 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.42708333333333331</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
test(connexion et partage des donnees via mqtt);  doc(Documentation Technique - BitTorrentMusic.md); fix(correction des bugs(connexion et partage des donnees via mqtt))
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NademoYosef.xlsx
+++ b/doc/Journal-de-Travail_NademoYosef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\BitTorrentMusic\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB47D7C-EF49-4FBF-836B-9EF03B313D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE792ED-20BC-49F6-A901-C16A34C9FC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="33855" yWindow="0" windowWidth="21600" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>Auteur:</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>correction des bugs(connexion et partage des donnees via mqtt)</t>
+  </si>
+  <si>
+    <t>Documentation Technique - BitTorrentMusic.md</t>
   </si>
 </sst>
 </file>
@@ -1284,13 +1287,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>670</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2217,13 +2220,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85350318471337583</c:v>
+                  <c:v>0.78527607361963192</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9108280254777069E-2</c:v>
+                  <c:v>1.8404907975460124E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12738853503184713</c:v>
+                  <c:v>0.19631901840490798</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4412,7 +4415,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4467,7 +4470,7 @@
       <c r="B3" s="92"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>13 heures 5 minutes</v>
+        <v>13 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4486,11 +4489,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>605</v>
+        <v>635</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>785</v>
+        <v>815</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5253,10 +5256,10 @@
       <c r="B39" s="34">
         <v>46010</v>
       </c>
-      <c r="C39" s="35">
-        <v>1</v>
-      </c>
-      <c r="D39" s="36"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="36">
+        <v>30</v>
+      </c>
       <c r="E39" s="37" t="s">
         <v>19</v>
       </c>
@@ -5266,15 +5269,23 @@
       <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="str">
+      <c r="A40" s="62">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31"/>
+        <v>51</v>
+      </c>
+      <c r="B40" s="30">
+        <v>46010</v>
+      </c>
+      <c r="C40" s="31">
+        <v>1</v>
+      </c>
       <c r="D40" s="32"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="22"/>
+      <c r="E40" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>67</v>
+      </c>
       <c r="G40" s="39"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -11365,15 +11376,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>670</v>
+        <v>640</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11381,11 +11392,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>11 h 10 min</v>
+        <v>10 h 40 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.85350318471337583</v>
+        <v>0.78527607361963192</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11422,7 +11433,7 @@
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>1.9108280254777069E-2</v>
+        <v>1.8404907975460124E-2</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11439,7 +11450,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
@@ -11447,7 +11458,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11455,11 +11466,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 40 min</v>
+        <v>2 h 40 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.12738853503184713</v>
+        <v>0.19631901840490798</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11515,22 +11526,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>605</v>
+        <v>635</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>785</v>
+        <v>815</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>13 h 05 min</v>
+        <v>13 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.54513888888888884</v>
+        <v>0.56597222222222221</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>